<commit_message>
Error redirect to /send
</commit_message>
<xml_diff>
--- a/python/exel/links.xlsx
+++ b/python/exel/links.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,12 +446,29 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2023-10-16 16:46:27</t>
+          <t>2023-10-16 18:06:27</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>172.24.0.1</t>
+          <t>172.29.0.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Bartek</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2023-10-16 18:16:00</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>192.168.16.1</t>
         </is>
       </c>
     </row>

</xml_diff>